<commit_message>
Changed the filepaths' format
</commit_message>
<xml_diff>
--- a/current_rate.xlsx
+++ b/current_rate.xlsx
@@ -1580,10 +1580,10 @@
         <v>75000</v>
       </c>
       <c r="V15" t="n">
-        <v>2988.007433333334</v>
+        <v>3259.174822222222</v>
       </c>
       <c r="W15" t="n">
-        <v>8.447192755792639</v>
+        <v>8.095961032197602</v>
       </c>
       <c r="X15" t="n">
         <v>10000</v>

</xml_diff>